<commit_message>
Report Generator Via Outlook
</commit_message>
<xml_diff>
--- a/Test_Execution_Report.xlsx
+++ b/Test_Execution_Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>Test_Case_Id</t>
   </si>
@@ -34,7 +34,7 @@
     <t>parameter</t>
   </si>
   <si>
-    <t>Test Case 1</t>
+    <t>Test Case 2</t>
   </si>
   <si>
     <t>Test Case 3</t>
@@ -43,10 +43,7 @@
     <t>Test Case 4</t>
   </si>
   <si>
-    <t>Test Case 6</t>
-  </si>
-  <si>
-    <t>Test Case 7</t>
+    <t>Test Case 8</t>
   </si>
   <si>
     <t>Test Case 9</t>
@@ -55,22 +52,25 @@
     <t>Test Case 10</t>
   </si>
   <si>
+    <t>Test Case 12</t>
+  </si>
+  <si>
     <t>Test Case 13</t>
   </si>
   <si>
-    <t>Test Case 14</t>
-  </si>
-  <si>
     <t>Test Case 15</t>
   </si>
   <si>
     <t>Test Case 17</t>
   </si>
   <si>
+    <t>Test Case 19</t>
+  </si>
+  <si>
     <t>Test Case 20</t>
   </si>
   <si>
-    <t>Test Case 22</t>
+    <t>Test Case 21</t>
   </si>
   <si>
     <t>Test Case 23</t>
@@ -79,12 +79,24 @@
     <t>Test Case 25</t>
   </si>
   <si>
+    <t>Test Case 26</t>
+  </si>
+  <si>
+    <t>Test Case 27</t>
+  </si>
+  <si>
+    <t>Test Case 28</t>
+  </si>
+  <si>
+    <t>Test Case 29</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Bank_Overview_Widget</t>
   </si>
   <si>
@@ -112,7 +124,13 @@
     <t>Portfolio_Health_Category_SMA1</t>
   </si>
   <si>
-    <t>Total_Outstandingamount</t>
+    <t>Portfolio_Health_Category_SMA2</t>
+  </si>
+  <si>
+    <t>Portfolio_Health_Category_NPA</t>
+  </si>
+  <si>
+    <t>Customers_count</t>
   </si>
   <si>
     <t>Active_Loans</t>
@@ -121,19 +139,19 @@
     <t>Total Outstanding</t>
   </si>
   <si>
-    <t>Active Loans</t>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Loans</t>
   </si>
   <si>
     <t>Loan disbursed</t>
   </si>
   <si>
-    <t>Loans</t>
-  </si>
-  <si>
-    <t>Customers</t>
-  </si>
-  <si>
     <t>OutStanding</t>
+  </si>
+  <si>
+    <t>Loans Disbursed</t>
   </si>
   <si>
     <t>Total Customers</t>
@@ -494,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,19 +543,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>4539016406.480292</v>
+        <v>251496</v>
       </c>
       <c r="C2">
-        <v>4539092685</v>
+        <v>251499</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -551,13 +569,13 @@
         <v>251499</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -565,19 +583,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>4539016406.480286</v>
+        <v>4539016406.480295</v>
       </c>
       <c r="C4">
         <v>4539092685</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -585,19 +603,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>251496</v>
+        <v>1051</v>
       </c>
       <c r="C5">
-        <v>251499</v>
+        <v>1046</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -605,19 +623,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>54583000</v>
+        <v>1051</v>
       </c>
       <c r="C6">
-        <v>50373000</v>
+        <v>1046</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -625,19 +643,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>1051</v>
+        <v>54583000</v>
       </c>
       <c r="C7">
-        <v>1046</v>
+        <v>50373000</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -645,19 +663,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>54583000</v>
+        <v>1051</v>
       </c>
       <c r="C8">
-        <v>50373000</v>
+        <v>1046</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -671,13 +689,13 @@
         <v>50373000</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -691,13 +709,13 @@
         <v>1046</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -705,19 +723,19 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>1051</v>
+        <v>4539016406.480296</v>
       </c>
       <c r="C11">
-        <v>1046</v>
+        <v>4539092685</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -725,19 +743,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>4539016406.480282</v>
+        <v>1837928000</v>
       </c>
       <c r="C12">
-        <v>4539092685</v>
+        <v>1802201000</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -745,19 +763,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>3317057243.480189</v>
+        <v>3317057243.480174</v>
       </c>
       <c r="C13">
         <v>3402313794</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -765,19 +783,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>219961755.4399991</v>
+        <v>188014</v>
       </c>
       <c r="C14">
-        <v>219990678</v>
+        <v>189809</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -791,13 +809,13 @@
         <v>14717</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -811,13 +829,93 @@
         <v>11246</v>
       </c>
       <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B17">
+        <v>106903206.86</v>
+      </c>
+      <c r="C17">
+        <v>106903299</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>6637</v>
+      </c>
+      <c r="C18">
+        <v>6637</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>720633169.6399996</v>
+      </c>
+      <c r="C19">
+        <v>720633275</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>30883</v>
+      </c>
+      <c r="C20">
+        <v>30883</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>